<commit_message>
udpated xlsx files issue  n.34
</commit_message>
<xml_diff>
--- a/data/coded_segments/aw_1_1.xlsx
+++ b/data/coded_segments/aw_1_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4098" windowHeight="3672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3143" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="907">
   <si>
     <t>Color</t>
   </si>
@@ -2831,6 +2831,60 @@
   </si>
   <si>
     <t>imepenem</t>
+  </si>
+  <si>
+    <t>1: 1660</t>
+  </si>
+  <si>
+    <t>1: 1663</t>
+  </si>
+  <si>
+    <t>dattaray</t>
+  </si>
+  <si>
+    <t>9/17/2019 11:38:55</t>
+  </si>
+  <si>
+    <t>1: 222</t>
+  </si>
+  <si>
+    <t>1: 226</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>9/17/2019 11:39:49</t>
+  </si>
+  <si>
+    <t>1: 214</t>
+  </si>
+  <si>
+    <t>Monza</t>
+  </si>
+  <si>
+    <t>9/17/2019 11:40:35</t>
+  </si>
+  <si>
+    <t>1: 156</t>
+  </si>
+  <si>
+    <t>1: 188</t>
+  </si>
+  <si>
+    <t>San Gerardo de’ Tintori” Hospital</t>
+  </si>
+  <si>
+    <t>9/17/2019 11:40:57</t>
+  </si>
+  <si>
+    <t>1: 454</t>
+  </si>
+  <si>
+    <t>1: 459</t>
+  </si>
+  <si>
+    <t>9/17/2019 11:41:56</t>
   </si>
 </sst>
 </file>
@@ -2845,19 +2899,16 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF909090"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -3264,9 +3315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M314"/>
+  <dimension ref="A1:M319"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -16153,6 +16206,211 @@
         <v>883</v>
       </c>
     </row>
+    <row r="315" spans="1:13" ht="15.6">
+      <c r="A315" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="G315" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="H315" s="3">
+        <v>0</v>
+      </c>
+      <c r="I315" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="J315" s="3">
+        <v>4</v>
+      </c>
+      <c r="K315" s="4">
+        <v>2.6444532592886424E-2</v>
+      </c>
+      <c r="L315" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="M315" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" ht="15.6">
+      <c r="A316" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F316" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="G316" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="H316" s="3">
+        <v>0</v>
+      </c>
+      <c r="I316" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="J316" s="3">
+        <v>5</v>
+      </c>
+      <c r="K316" s="4">
+        <v>4.4385264092321346E-2</v>
+      </c>
+      <c r="L316" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="M316" s="1" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" ht="15.6">
+      <c r="A317" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G317" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="H317" s="3">
+        <v>0</v>
+      </c>
+      <c r="I317" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="J317" s="3">
+        <v>5</v>
+      </c>
+      <c r="K317" s="4">
+        <v>4.4385264092321346E-2</v>
+      </c>
+      <c r="L317" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="M317" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" ht="15.6">
+      <c r="A318" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D318" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="G318" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="H318" s="3">
+        <v>0</v>
+      </c>
+      <c r="I318" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="J318" s="3">
+        <v>33</v>
+      </c>
+      <c r="K318" s="4">
+        <v>0.29294274300932088</v>
+      </c>
+      <c r="L318" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="M318" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" ht="15.6">
+      <c r="A319" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="G319" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="H319" s="3">
+        <v>0</v>
+      </c>
+      <c r="I319" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="J319" s="3">
+        <v>6</v>
+      </c>
+      <c r="K319" s="4">
+        <v>2.7466239414053559E-2</v>
+      </c>
+      <c r="L319" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="M319" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>